<commit_message>
Functionalized repetitive codeblocks in main()
</commit_message>
<xml_diff>
--- a/ByHand_Figures.xlsx
+++ b/ByHand_Figures.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gjang\Documents\GitHub\CAI-Analysis-Script\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D54FD36E-FC2C-4A6F-A6B1-76AE2BFA1868}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{112BA3E8-65B8-493B-935D-3AF1C8199705}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5256" yWindow="3060" windowWidth="16584" windowHeight="9900" activeTab="1" xr2:uid="{75C88B91-9FDD-4DAF-A44D-494ABB0DD9AA}"/>
+    <workbookView xWindow="828" yWindow="-108" windowWidth="22320" windowHeight="13176" activeTab="1" xr2:uid="{75C88B91-9FDD-4DAF-A44D-494ABB0DD9AA}"/>
   </bookViews>
   <sheets>
     <sheet name="Tiznado-Hernandez" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="35">
   <si>
     <t>All</t>
   </si>
@@ -122,6 +122,24 @@
   </si>
   <si>
     <t>Experimental vs.  Theoretical Area</t>
+  </si>
+  <si>
+    <t>Threshold</t>
+  </si>
+  <si>
+    <t>Current Analysis</t>
+  </si>
+  <si>
+    <t>Tiznado-Hernandez et. al.</t>
+  </si>
+  <si>
+    <t>Adj. R^2 by Threshold</t>
+  </si>
+  <si>
+    <t>P-Value by Threshold</t>
+  </si>
+  <si>
+    <t>Reis Model/R^2</t>
   </si>
 </sst>
 </file>
@@ -265,7 +283,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="36">
+  <borders count="50">
     <border>
       <left/>
       <right/>
@@ -674,11 +692,171 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="92">
+  <cellXfs count="119">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
@@ -758,12 +936,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -815,6 +987,55 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="2" borderId="39" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="12" borderId="39" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="13" borderId="39" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="14" borderId="39" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="15" borderId="39" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="16" borderId="39" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="17" borderId="39" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="18" borderId="39" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="19" borderId="39" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="11" borderId="45" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="20" borderId="46" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1143,10 +1364,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF204F42-1E92-4DBB-A3DF-20144B547879}">
-  <dimension ref="A1:O39"/>
+  <dimension ref="A1:W39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K6" sqref="K6:O25"/>
+    <sheetView topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="R5" sqref="R5:W25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1156,9 +1377,13 @@
     <col min="3" max="3" width="10.88671875" customWidth="1"/>
     <col min="5" max="5" width="9.5546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="10" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.77734375" customWidth="1"/>
+    <col min="19" max="19" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="10" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="8.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>4</v>
       </c>
@@ -1169,7 +1394,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1180,7 +1405,7 @@
         <v>1E-4</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1191,7 +1416,8 @@
         <v>1E-4</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="5" spans="1:23" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>1</v>
       </c>
@@ -1200,8 +1426,22 @@
       <c r="M5" s="41"/>
       <c r="N5" s="40"/>
       <c r="O5" s="41"/>
-    </row>
-    <row r="6" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="R5" s="113" t="s">
+        <v>31</v>
+      </c>
+      <c r="S5" s="114" t="s">
+        <v>6</v>
+      </c>
+      <c r="T5" s="93" t="s">
+        <v>4</v>
+      </c>
+      <c r="U5" s="93"/>
+      <c r="V5" s="93" t="s">
+        <v>27</v>
+      </c>
+      <c r="W5" s="94"/>
+    </row>
+    <row r="6" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -1214,13 +1454,21 @@
       <c r="L6" s="71" t="s">
         <v>5</v>
       </c>
-      <c r="M6" s="72"/>
+      <c r="M6" s="71"/>
       <c r="N6" s="71" t="s">
         <v>27</v>
       </c>
-      <c r="O6" s="73"/>
-    </row>
-    <row r="7" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="O6" s="90"/>
+      <c r="R6" s="115"/>
+      <c r="S6" s="91"/>
+      <c r="T6" s="80" t="s">
+        <v>28</v>
+      </c>
+      <c r="U6" s="81"/>
+      <c r="V6" s="81"/>
+      <c r="W6" s="95"/>
+    </row>
+    <row r="7" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -1241,14 +1489,26 @@
       <c r="K7" s="62" t="s">
         <v>9</v>
       </c>
-      <c r="L7" s="82" t="s">
+      <c r="L7" s="80" t="s">
         <v>28</v>
       </c>
-      <c r="M7" s="83"/>
-      <c r="N7" s="83"/>
-      <c r="O7" s="84"/>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="M7" s="81"/>
+      <c r="N7" s="81"/>
+      <c r="O7" s="82"/>
+      <c r="R7" s="115"/>
+      <c r="S7" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="T7" s="74">
+        <v>0.9637</v>
+      </c>
+      <c r="U7" s="75"/>
+      <c r="V7" s="74">
+        <v>1E-4</v>
+      </c>
+      <c r="W7" s="96"/>
+    </row>
+    <row r="8" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>242</v>
       </c>
@@ -1269,16 +1529,28 @@
       <c r="K8" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="L8" s="76">
+      <c r="L8" s="74">
         <v>0.9637</v>
       </c>
-      <c r="M8" s="77"/>
+      <c r="M8" s="75"/>
       <c r="N8" s="74">
         <v>1E-4</v>
       </c>
-      <c r="O8" s="75"/>
-    </row>
-    <row r="9" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="O8" s="73"/>
+      <c r="R8" s="115"/>
+      <c r="S8" s="92" t="s">
+        <v>3</v>
+      </c>
+      <c r="T8" s="76">
+        <v>0.94499999999999995</v>
+      </c>
+      <c r="U8" s="77"/>
+      <c r="V8" s="78">
+        <v>1E-4</v>
+      </c>
+      <c r="W8" s="97"/>
+    </row>
+    <row r="9" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>246</v>
       </c>
@@ -1299,16 +1571,28 @@
       <c r="K9" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="L9" s="78">
+      <c r="L9" s="76">
         <v>0.94499999999999995</v>
       </c>
-      <c r="M9" s="79"/>
-      <c r="N9" s="80">
+      <c r="M9" s="77"/>
+      <c r="N9" s="78">
         <v>1E-4</v>
       </c>
-      <c r="O9" s="81"/>
-    </row>
-    <row r="10" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="O9" s="79"/>
+      <c r="R9" s="115" t="s">
+        <v>30</v>
+      </c>
+      <c r="S9" s="3"/>
+      <c r="T9" s="72" t="s">
+        <v>32</v>
+      </c>
+      <c r="U9" s="72"/>
+      <c r="V9" s="72" t="s">
+        <v>33</v>
+      </c>
+      <c r="W9" s="98"/>
+    </row>
+    <row r="10" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>319</v>
       </c>
@@ -1341,8 +1625,24 @@
       <c r="O10" s="70">
         <v>0.95</v>
       </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="R10" s="115"/>
+      <c r="S10" s="91" t="s">
+        <v>29</v>
+      </c>
+      <c r="T10" s="67">
+        <v>1</v>
+      </c>
+      <c r="U10" s="68">
+        <v>0.95</v>
+      </c>
+      <c r="V10" s="69">
+        <v>1</v>
+      </c>
+      <c r="W10" s="99">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>325</v>
       </c>
@@ -1375,8 +1675,24 @@
       <c r="O11" s="43">
         <v>2.2E-16</v>
       </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="R11" s="115"/>
+      <c r="S11" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="T11" s="15">
+        <v>0.88241720000000001</v>
+      </c>
+      <c r="U11" s="65">
+        <v>0.89288350000000005</v>
+      </c>
+      <c r="V11" s="42">
+        <v>2.2E-16</v>
+      </c>
+      <c r="W11" s="100">
+        <v>2.2E-16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>326</v>
       </c>
@@ -1409,8 +1725,24 @@
       <c r="O12" s="43">
         <v>2.2E-16</v>
       </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="R12" s="115"/>
+      <c r="S12" s="3">
+        <v>242</v>
+      </c>
+      <c r="T12" s="15">
+        <v>0.97212770000000004</v>
+      </c>
+      <c r="U12" s="65">
+        <v>0.9859424</v>
+      </c>
+      <c r="V12" s="42">
+        <v>2.2E-16</v>
+      </c>
+      <c r="W12" s="100">
+        <v>2.2E-16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>390</v>
       </c>
@@ -1443,8 +1775,24 @@
       <c r="O13" s="43">
         <v>2.2E-16</v>
       </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="R13" s="115"/>
+      <c r="S13" s="3">
+        <v>246</v>
+      </c>
+      <c r="T13" s="15">
+        <v>0.86197349999999995</v>
+      </c>
+      <c r="U13" s="65">
+        <v>0.92972060000000001</v>
+      </c>
+      <c r="V13" s="44">
+        <v>1.1880000000000001E-14</v>
+      </c>
+      <c r="W13" s="100">
+        <v>2.2E-16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>572</v>
       </c>
@@ -1477,8 +1825,24 @@
       <c r="O14" s="46">
         <v>4.4770000000000001E-3</v>
       </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="R14" s="115"/>
+      <c r="S14" s="3">
+        <v>319</v>
+      </c>
+      <c r="T14" s="15">
+        <v>0.27889419999999998</v>
+      </c>
+      <c r="U14" s="65">
+        <v>0.22075339999999999</v>
+      </c>
+      <c r="V14" s="45">
+        <v>1.119E-3</v>
+      </c>
+      <c r="W14" s="101">
+        <v>4.4770000000000001E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>580</v>
       </c>
@@ -1511,8 +1875,24 @@
       <c r="O15" s="47">
         <v>3.4309999999999999E-16</v>
       </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="R15" s="115"/>
+      <c r="S15" s="3">
+        <v>325</v>
+      </c>
+      <c r="T15" s="15">
+        <v>0.90736779999999995</v>
+      </c>
+      <c r="U15" s="65">
+        <v>0.90705380000000002</v>
+      </c>
+      <c r="V15" s="42">
+        <v>2.2E-16</v>
+      </c>
+      <c r="W15" s="102">
+        <v>3.4309999999999999E-16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>582</v>
       </c>
@@ -1545,8 +1925,24 @@
       <c r="O16" s="43">
         <v>2.2E-16</v>
       </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="R16" s="115"/>
+      <c r="S16" s="3">
+        <v>326</v>
+      </c>
+      <c r="T16" s="15">
+        <v>0.92248249999999998</v>
+      </c>
+      <c r="U16" s="65">
+        <v>0.92471369999999997</v>
+      </c>
+      <c r="V16" s="42">
+        <v>2.2E-16</v>
+      </c>
+      <c r="W16" s="100">
+        <v>2.2E-16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>584</v>
       </c>
@@ -1579,8 +1975,25 @@
       <c r="O17" s="49">
         <v>7.1849999999999998E-12</v>
       </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="Q17" s="118"/>
+      <c r="R17" s="115"/>
+      <c r="S17" s="3">
+        <v>390</v>
+      </c>
+      <c r="T17" s="15">
+        <v>0.8139748</v>
+      </c>
+      <c r="U17" s="65">
+        <v>0.81148540000000002</v>
+      </c>
+      <c r="V17" s="48">
+        <v>1.071E-12</v>
+      </c>
+      <c r="W17" s="103">
+        <v>7.1849999999999998E-12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>585</v>
       </c>
@@ -1613,8 +2026,24 @@
       <c r="O18" s="51">
         <v>3.3330000000000003E-11</v>
       </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="R18" s="115"/>
+      <c r="S18" s="3">
+        <v>572</v>
+      </c>
+      <c r="T18" s="15">
+        <v>0.78859900000000005</v>
+      </c>
+      <c r="U18" s="65">
+        <v>0.78982699999999995</v>
+      </c>
+      <c r="V18" s="50">
+        <v>7.3970000000000001E-12</v>
+      </c>
+      <c r="W18" s="104">
+        <v>3.3330000000000003E-11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>839</v>
       </c>
@@ -1647,8 +2076,24 @@
       <c r="O19" s="53">
         <v>3.354E-12</v>
       </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="R19" s="115"/>
+      <c r="S19" s="3">
+        <v>580</v>
+      </c>
+      <c r="T19" s="15">
+        <v>0.83496899999999996</v>
+      </c>
+      <c r="U19" s="65">
+        <v>0.81032559999999998</v>
+      </c>
+      <c r="V19" s="52">
+        <v>1.757E-13</v>
+      </c>
+      <c r="W19" s="105">
+        <v>3.354E-12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>845</v>
       </c>
@@ -1681,8 +2126,24 @@
       <c r="O20" s="55">
         <v>2.8699999999999999E-13</v>
       </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="R20" s="115"/>
+      <c r="S20" s="3">
+        <v>582</v>
+      </c>
+      <c r="T20" s="15">
+        <v>0.82477900000000004</v>
+      </c>
+      <c r="U20" s="65">
+        <v>0.85000240000000005</v>
+      </c>
+      <c r="V20" s="54">
+        <v>4.3409999999999999E-13</v>
+      </c>
+      <c r="W20" s="106">
+        <v>2.8699999999999999E-13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>854</v>
       </c>
@@ -1715,8 +2176,24 @@
       <c r="O21" s="43">
         <v>2.2E-16</v>
       </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="R21" s="115"/>
+      <c r="S21" s="3">
+        <v>584</v>
+      </c>
+      <c r="T21" s="15">
+        <v>0.96065520000000004</v>
+      </c>
+      <c r="U21" s="65">
+        <v>0.96058759999999999</v>
+      </c>
+      <c r="V21" s="42">
+        <v>2.2E-16</v>
+      </c>
+      <c r="W21" s="100">
+        <v>2.2E-16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:23" x14ac:dyDescent="0.3">
       <c r="K22" s="2">
         <v>585</v>
       </c>
@@ -1732,8 +2209,24 @@
       <c r="O22" s="57">
         <v>3.2889999999999999E-8</v>
       </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="R22" s="115"/>
+      <c r="S22" s="3">
+        <v>585</v>
+      </c>
+      <c r="T22" s="15">
+        <v>0.58418490000000001</v>
+      </c>
+      <c r="U22" s="65">
+        <v>0.64494130000000005</v>
+      </c>
+      <c r="V22" s="56">
+        <v>2.1509999999999999E-7</v>
+      </c>
+      <c r="W22" s="107">
+        <v>3.2889999999999999E-8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>0.95</v>
       </c>
@@ -1752,8 +2245,24 @@
       <c r="O23" s="59">
         <v>1.61E-12</v>
       </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="R23" s="115"/>
+      <c r="S23" s="3">
+        <v>839</v>
+      </c>
+      <c r="T23" s="15">
+        <v>0.7474227</v>
+      </c>
+      <c r="U23" s="65">
+        <v>0.83046549999999997</v>
+      </c>
+      <c r="V23" s="58">
+        <v>2.2109999999999999E-10</v>
+      </c>
+      <c r="W23" s="108">
+        <v>1.61E-12</v>
+      </c>
+    </row>
+    <row r="24" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>6</v>
       </c>
@@ -1775,8 +2284,24 @@
       <c r="O24" s="43">
         <v>2.2E-16</v>
       </c>
-    </row>
-    <row r="25" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="R24" s="115"/>
+      <c r="S24" s="3">
+        <v>845</v>
+      </c>
+      <c r="T24" s="15">
+        <v>0.9407894</v>
+      </c>
+      <c r="U24" s="65">
+        <v>0.93803709999999996</v>
+      </c>
+      <c r="V24" s="42">
+        <v>2.2E-16</v>
+      </c>
+      <c r="W24" s="100">
+        <v>2.2E-16</v>
+      </c>
+    </row>
+    <row r="25" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>0</v>
       </c>
@@ -1816,8 +2341,24 @@
       <c r="O25" s="61">
         <v>1.0579999999999999E-3</v>
       </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="R25" s="116"/>
+      <c r="S25" s="117">
+        <v>854</v>
+      </c>
+      <c r="T25" s="109">
+        <v>0.29161949999999998</v>
+      </c>
+      <c r="U25" s="110">
+        <v>0.28973280000000001</v>
+      </c>
+      <c r="V25" s="111">
+        <v>8.4230000000000004E-4</v>
+      </c>
+      <c r="W25" s="112">
+        <v>1.0579999999999999E-3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>242</v>
       </c>
@@ -1843,7 +2384,7 @@
         <v>15.657577319177793</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>246</v>
       </c>
@@ -1869,7 +2410,7 @@
         <v>15.657577319177793</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>319</v>
       </c>
@@ -1895,7 +2436,7 @@
         <v>2.3490129056165547</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>325</v>
       </c>
@@ -1921,7 +2462,7 @@
         <v>15.464579281943827</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>326</v>
       </c>
@@ -1947,7 +2488,7 @@
         <v>15.657577319177793</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>390</v>
       </c>
@@ -1973,7 +2514,7 @@
         <v>11.143573227529755</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>572</v>
       </c>
@@ -2182,7 +2723,18 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="18">
+    <mergeCell ref="T8:U8"/>
+    <mergeCell ref="V8:W8"/>
+    <mergeCell ref="T9:U9"/>
+    <mergeCell ref="V9:W9"/>
+    <mergeCell ref="R9:R25"/>
+    <mergeCell ref="R5:R8"/>
+    <mergeCell ref="T5:U5"/>
+    <mergeCell ref="V5:W5"/>
+    <mergeCell ref="T6:W6"/>
+    <mergeCell ref="T7:U7"/>
+    <mergeCell ref="V7:W7"/>
     <mergeCell ref="L6:M6"/>
     <mergeCell ref="N6:O6"/>
     <mergeCell ref="N8:O8"/>
@@ -2192,7 +2744,7 @@
     <mergeCell ref="L7:O7"/>
   </mergeCells>
   <conditionalFormatting sqref="B2:B3">
-    <cfRule type="colorScale" priority="11">
+    <cfRule type="colorScale" priority="15">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="0.5"/>
@@ -2204,6 +2756,54 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B25:B39">
+    <cfRule type="colorScale" priority="13">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="0.5"/>
+        <cfvo type="num" val="1"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B7:B21">
+    <cfRule type="colorScale" priority="14">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="0.5"/>
+        <cfvo type="num" val="1"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E7:E21">
+    <cfRule type="colorScale" priority="11">
+      <colorScale>
+        <cfvo type="num" val="1"/>
+        <cfvo type="num" val="4"/>
+        <cfvo type="num" val="15.657579999999999"/>
+        <color rgb="FFFFC000"/>
+        <color theme="0"/>
+        <color rgb="FF00B0F0"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25:E39">
+    <cfRule type="colorScale" priority="10">
+      <colorScale>
+        <cfvo type="num" val="1"/>
+        <cfvo type="num" val="4"/>
+        <cfvo type="num" val="15.657579999999999"/>
+        <color rgb="FFFFC000"/>
+        <color theme="0"/>
+        <color rgb="FF00B0F0"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L11:L25">
     <cfRule type="colorScale" priority="9">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -2215,8 +2815,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B7:B21">
-    <cfRule type="colorScale" priority="10">
+  <conditionalFormatting sqref="M11:M25">
+    <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="0.5"/>
@@ -2227,31 +2827,19 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E7:E21">
+  <conditionalFormatting sqref="L8">
     <cfRule type="colorScale" priority="7">
       <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="0.5"/>
         <cfvo type="num" val="1"/>
-        <cfvo type="num" val="4"/>
-        <cfvo type="num" val="15.657579999999999"/>
-        <color rgb="FFFFC000"/>
-        <color theme="0"/>
-        <color rgb="FF00B0F0"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E25:E39">
-    <cfRule type="colorScale" priority="6">
-      <colorScale>
-        <cfvo type="num" val="1"/>
-        <cfvo type="num" val="4"/>
-        <cfvo type="num" val="15.657579999999999"/>
-        <color rgb="FFFFC000"/>
-        <color theme="0"/>
-        <color rgb="FF00B0F0"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L11:L25">
+  <conditionalFormatting sqref="L9">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -2263,7 +2851,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M11:M25">
+  <conditionalFormatting sqref="T11:T25">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -2275,7 +2863,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L8">
+  <conditionalFormatting sqref="U11:U25">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -2287,7 +2875,19 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L9">
+  <conditionalFormatting sqref="T7">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="0.5"/>
+        <cfvo type="num" val="1"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="T8">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -2308,8 +2908,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEBA3CFB-F8B2-4C6A-A42E-E104C75F3ED9}">
   <dimension ref="A3:U67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F16" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="T48" sqref="T48"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="J50" sqref="J50:N67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2322,7 +2922,7 @@
     <col min="9" max="9" width="12.5546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11.21875" bestFit="1" customWidth="1"/>
     <col min="11" max="13" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:18" x14ac:dyDescent="0.3">
@@ -2344,11 +2944,11 @@
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="J7" s="85"/>
-      <c r="K7" s="85"/>
-      <c r="L7" s="85"/>
-      <c r="M7" s="85"/>
-      <c r="N7" s="85"/>
+      <c r="J7" s="83"/>
+      <c r="K7" s="83"/>
+      <c r="L7" s="83"/>
+      <c r="M7" s="83"/>
+      <c r="N7" s="83"/>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="C8" t="s">
@@ -2366,13 +2966,13 @@
       <c r="J8" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="K8" s="89" t="s">
+      <c r="K8" s="87" t="s">
         <v>25</v>
       </c>
-      <c r="L8" s="90"/>
-      <c r="M8" s="91"/>
+      <c r="L8" s="88"/>
+      <c r="M8" s="89"/>
       <c r="N8" s="14" t="s">
-        <v>9</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -2429,7 +3029,7 @@
       <c r="M10" s="9">
         <v>0.88464969999999998</v>
       </c>
-      <c r="N10" s="86">
+      <c r="N10" s="84">
         <v>0.91</v>
       </c>
       <c r="P10" s="15">
@@ -2467,7 +3067,7 @@
       <c r="M11" s="4">
         <v>0.97865310000000005</v>
       </c>
-      <c r="N11" s="87"/>
+      <c r="N11" s="85"/>
       <c r="P11" s="15">
         <v>246</v>
       </c>
@@ -2503,7 +3103,7 @@
       <c r="M12" s="4">
         <v>0.88532860000000002</v>
       </c>
-      <c r="N12" s="87"/>
+      <c r="N12" s="85"/>
       <c r="P12" s="15">
         <v>319</v>
       </c>
@@ -2539,7 +3139,7 @@
       <c r="M13" s="4">
         <v>0.53159990000000001</v>
       </c>
-      <c r="N13" s="87"/>
+      <c r="N13" s="85"/>
       <c r="P13" s="15">
         <v>325</v>
       </c>
@@ -2575,7 +3175,7 @@
       <c r="M14" s="4">
         <v>0.90210449999999998</v>
       </c>
-      <c r="N14" s="87"/>
+      <c r="N14" s="85"/>
       <c r="P14" s="15">
         <v>326</v>
       </c>
@@ -2611,7 +3211,7 @@
       <c r="M15" s="4">
         <v>0.93822689999999997</v>
       </c>
-      <c r="N15" s="87"/>
+      <c r="N15" s="85"/>
       <c r="P15" s="15">
         <v>390</v>
       </c>
@@ -2647,7 +3247,7 @@
       <c r="M16" s="4">
         <v>0.80340739999999999</v>
       </c>
-      <c r="N16" s="87"/>
+      <c r="N16" s="85"/>
       <c r="P16" s="15">
         <v>572</v>
       </c>
@@ -2683,7 +3283,7 @@
       <c r="M17" s="4">
         <v>0.89299620000000002</v>
       </c>
-      <c r="N17" s="87"/>
+      <c r="N17" s="85"/>
       <c r="P17" s="15">
         <v>580</v>
       </c>
@@ -2719,7 +3319,7 @@
       <c r="M18" s="4">
         <v>0.82649229999999996</v>
       </c>
-      <c r="N18" s="87"/>
+      <c r="N18" s="85"/>
       <c r="P18" s="15">
         <v>582</v>
       </c>
@@ -2755,7 +3355,7 @@
       <c r="M19" s="4">
         <v>0.83606809999999998</v>
       </c>
-      <c r="N19" s="87"/>
+      <c r="N19" s="85"/>
       <c r="P19" s="15">
         <v>584</v>
       </c>
@@ -2791,7 +3391,7 @@
       <c r="M20" s="4">
         <v>0.95969510000000002</v>
       </c>
-      <c r="N20" s="87"/>
+      <c r="N20" s="85"/>
       <c r="P20" s="15">
         <v>585</v>
       </c>
@@ -2827,7 +3427,7 @@
       <c r="M21" s="4">
         <v>0.63227610000000001</v>
       </c>
-      <c r="N21" s="87"/>
+      <c r="N21" s="85"/>
       <c r="P21" s="15">
         <v>839</v>
       </c>
@@ -2863,7 +3463,7 @@
       <c r="M22" s="4">
         <v>0.93453529999999996</v>
       </c>
-      <c r="N22" s="87"/>
+      <c r="N22" s="85"/>
       <c r="P22" s="15">
         <v>845</v>
       </c>
@@ -2899,7 +3499,7 @@
       <c r="M23" s="4">
         <v>0.96714650000000002</v>
       </c>
-      <c r="N23" s="87"/>
+      <c r="N23" s="85"/>
       <c r="P23" s="15">
         <v>854</v>
       </c>
@@ -2935,7 +3535,7 @@
       <c r="M24" s="4">
         <v>0.30718679999999998</v>
       </c>
-      <c r="N24" s="87"/>
+      <c r="N24" s="85"/>
     </row>
     <row r="25" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B25" t="s">
@@ -2968,7 +3568,7 @@
         <f>AVERAGE(M11:M24)</f>
         <v>0.81397977142857147</v>
       </c>
-      <c r="N25" s="88"/>
+      <c r="N25" s="86"/>
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
@@ -3001,13 +3601,13 @@
       <c r="J29" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="K29" s="90" t="s">
+      <c r="K29" s="88" t="s">
         <v>25</v>
       </c>
-      <c r="L29" s="90"/>
-      <c r="M29" s="91"/>
+      <c r="L29" s="88"/>
+      <c r="M29" s="89"/>
       <c r="N29" s="14" t="s">
-        <v>9</v>
+        <v>34</v>
       </c>
     </row>
     <row r="30" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -3058,7 +3658,7 @@
       <c r="M31" s="9">
         <v>0.92971550000000003</v>
       </c>
-      <c r="N31" s="86">
+      <c r="N31" s="84">
         <v>0.91</v>
       </c>
       <c r="U31">
@@ -3090,7 +3690,7 @@
       <c r="M32" s="4">
         <v>0.97515470000000004</v>
       </c>
-      <c r="N32" s="87"/>
+      <c r="N32" s="85"/>
       <c r="U32">
         <v>390</v>
       </c>
@@ -3120,7 +3720,7 @@
       <c r="M33" s="4">
         <v>0.86565619999999999</v>
       </c>
-      <c r="N33" s="87"/>
+      <c r="N33" s="85"/>
       <c r="U33">
         <v>845</v>
       </c>
@@ -3150,7 +3750,7 @@
       <c r="M34" s="4">
         <v>0.84233049999999998</v>
       </c>
-      <c r="N34" s="87"/>
+      <c r="N34" s="85"/>
     </row>
     <row r="35" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B35">
@@ -3177,7 +3777,7 @@
       <c r="M35" s="4">
         <v>0.86612060000000002</v>
       </c>
-      <c r="N35" s="87"/>
+      <c r="N35" s="85"/>
     </row>
     <row r="36" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B36">
@@ -3204,7 +3804,7 @@
       <c r="M36" s="4">
         <v>0.91505349999999996</v>
       </c>
-      <c r="N36" s="87"/>
+      <c r="N36" s="85"/>
     </row>
     <row r="37" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B37">
@@ -3231,7 +3831,7 @@
       <c r="M37" s="4">
         <v>0.92223440000000001</v>
       </c>
-      <c r="N37" s="87"/>
+      <c r="N37" s="85"/>
     </row>
     <row r="38" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B38">
@@ -3258,7 +3858,7 @@
       <c r="M38" s="4">
         <v>0.75558380000000003</v>
       </c>
-      <c r="N38" s="87"/>
+      <c r="N38" s="85"/>
     </row>
     <row r="39" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B39">
@@ -3285,7 +3885,7 @@
       <c r="M39" s="4">
         <v>0.84381260000000002</v>
       </c>
-      <c r="N39" s="87"/>
+      <c r="N39" s="85"/>
     </row>
     <row r="40" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B40">
@@ -3312,7 +3912,7 @@
       <c r="M40" s="4">
         <v>0.84298899999999999</v>
       </c>
-      <c r="N40" s="87"/>
+      <c r="N40" s="85"/>
     </row>
     <row r="41" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B41">
@@ -3339,7 +3939,7 @@
       <c r="M41" s="4">
         <v>0.95335910000000001</v>
       </c>
-      <c r="N41" s="87"/>
+      <c r="N41" s="85"/>
     </row>
     <row r="42" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B42">
@@ -3366,7 +3966,7 @@
       <c r="M42" s="4">
         <v>0.86469220000000002</v>
       </c>
-      <c r="N42" s="87"/>
+      <c r="N42" s="85"/>
     </row>
     <row r="43" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B43">
@@ -3393,7 +3993,7 @@
       <c r="M43" s="4">
         <v>0.85319020000000001</v>
       </c>
-      <c r="N43" s="87"/>
+      <c r="N43" s="85"/>
     </row>
     <row r="44" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B44">
@@ -3420,7 +4020,7 @@
       <c r="M44" s="4">
         <v>0.9084354</v>
       </c>
-      <c r="N44" s="87"/>
+      <c r="N44" s="85"/>
     </row>
     <row r="45" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B45">
@@ -3447,7 +4047,7 @@
       <c r="M45" s="4">
         <v>0.81576859999999995</v>
       </c>
-      <c r="N45" s="87"/>
+      <c r="N45" s="85"/>
     </row>
     <row r="46" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B46" t="s">
@@ -3480,7 +4080,7 @@
         <f>AVERAGE(M32:M45)</f>
         <v>0.87317005714285723</v>
       </c>
-      <c r="N46" s="88"/>
+      <c r="N46" s="86"/>
     </row>
     <row r="47" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
@@ -3513,13 +4113,13 @@
       <c r="J50" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="K50" s="89" t="s">
+      <c r="K50" s="87" t="s">
         <v>25</v>
       </c>
-      <c r="L50" s="90"/>
-      <c r="M50" s="91"/>
+      <c r="L50" s="88"/>
+      <c r="M50" s="89"/>
       <c r="N50" s="14" t="s">
-        <v>9</v>
+        <v>34</v>
       </c>
     </row>
     <row r="51" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -3570,7 +4170,7 @@
       <c r="M52" s="9">
         <v>0.86650640000000001</v>
       </c>
-      <c r="N52" s="86">
+      <c r="N52" s="84">
         <v>0.72</v>
       </c>
       <c r="P52">
@@ -3609,7 +4209,7 @@
       <c r="M53" s="4">
         <v>0.97515470000000004</v>
       </c>
-      <c r="N53" s="87"/>
+      <c r="N53" s="85"/>
       <c r="P53">
         <v>0.97442341302618796</v>
       </c>
@@ -3650,7 +4250,7 @@
       <c r="M54" s="4">
         <v>0.86565619999999999</v>
       </c>
-      <c r="N54" s="87"/>
+      <c r="N54" s="85"/>
       <c r="P54">
         <v>0.90678652173858898</v>
       </c>
@@ -3691,7 +4291,7 @@
       <c r="M55" s="4">
         <v>0.84233049999999998</v>
       </c>
-      <c r="N55" s="87"/>
+      <c r="N55" s="85"/>
       <c r="P55">
         <v>0.84028026306244596</v>
       </c>
@@ -3732,7 +4332,7 @@
       <c r="M56" s="4">
         <v>0.86612060000000002</v>
       </c>
-      <c r="N56" s="87"/>
+      <c r="N56" s="85"/>
       <c r="P56">
         <v>0.86728205443133299</v>
       </c>
@@ -3773,7 +4373,7 @@
       <c r="M57" s="4">
         <v>0.91505349999999996</v>
       </c>
-      <c r="N57" s="87"/>
+      <c r="N57" s="85"/>
       <c r="P57">
         <v>0.92802743019062095</v>
       </c>
@@ -3814,7 +4414,7 @@
       <c r="M58" s="4">
         <v>0.92223440000000001</v>
       </c>
-      <c r="N58" s="87"/>
+      <c r="N58" s="85"/>
       <c r="P58">
         <v>0.92735345361697197</v>
       </c>
@@ -3855,7 +4455,7 @@
       <c r="M59" s="4">
         <v>0.75558380000000003</v>
       </c>
-      <c r="N59" s="87"/>
+      <c r="N59" s="85"/>
       <c r="P59">
         <v>0.79879974429663803</v>
       </c>
@@ -3896,7 +4496,7 @@
       <c r="M60" s="4">
         <v>0.84381260000000002</v>
       </c>
-      <c r="N60" s="87"/>
+      <c r="N60" s="85"/>
       <c r="P60">
         <v>0.82785920893316201</v>
       </c>
@@ -3937,7 +4537,7 @@
       <c r="M61" s="4">
         <v>0.84298899999999999</v>
       </c>
-      <c r="N61" s="87"/>
+      <c r="N61" s="85"/>
       <c r="P61">
         <v>0.85540101722200501</v>
       </c>
@@ -3978,7 +4578,7 @@
       <c r="M62" s="4">
         <v>0.95335910000000001</v>
       </c>
-      <c r="N62" s="87"/>
+      <c r="N62" s="85"/>
       <c r="P62">
         <v>0.95263232100741901</v>
       </c>
@@ -4019,7 +4619,7 @@
       <c r="M63" s="4">
         <v>0.86469220000000002</v>
       </c>
-      <c r="N63" s="87"/>
+      <c r="N63" s="85"/>
       <c r="P63">
         <v>0.86217247732360003</v>
       </c>
@@ -4060,7 +4660,7 @@
       <c r="M64" s="4">
         <v>0.85319020000000001</v>
       </c>
-      <c r="N64" s="87"/>
+      <c r="N64" s="85"/>
       <c r="P64">
         <v>0.88434330759582502</v>
       </c>
@@ -4101,7 +4701,7 @@
       <c r="M65" s="4">
         <v>0.9084354</v>
       </c>
-      <c r="N65" s="87"/>
+      <c r="N65" s="85"/>
       <c r="P65">
         <v>0.90181953709684803</v>
       </c>
@@ -4142,7 +4742,7 @@
       <c r="M66" s="4">
         <v>0.81576859999999995</v>
       </c>
-      <c r="N66" s="87"/>
+      <c r="N66" s="85"/>
       <c r="P66">
         <v>0.82314309599953495</v>
       </c>
@@ -4189,7 +4789,7 @@
         <f>AVERAGE(M53:M66)</f>
         <v>0.87317005714285723</v>
       </c>
-      <c r="N67" s="88"/>
+      <c r="N67" s="86"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>